<commit_message>
agrega imagenes y ejemplos de buenos y malos resultados
</commit_message>
<xml_diff>
--- a/resultados_magic_loop.xlsx
+++ b/resultados_magic_loop.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhnk7\Documents\MarioHeredia\ITAM\02_segundo_semestre\metodos_analiticos\final_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2834FCDA-1BB0-48FB-9139-CF247DE310B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A199E400-67BB-4B34-BFA9-4B2319807862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3DEE28E-3B65-4326-AC3A-6EBCD7C32232}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3DEE28E-3B65-4326-AC3A-6EBCD7C32232}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="good job example" sheetId="2" r:id="rId2"/>
+    <sheet name="bad job example" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$21:$E$31</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>alpha</t>
   </si>
@@ -52,14 +54,160 @@
   </si>
   <si>
     <t>Factores</t>
+  </si>
+  <si>
+    <t>app_name</t>
+  </si>
+  <si>
+    <t>CounterStrike</t>
+  </si>
+  <si>
+    <t>Team Fortress 2</t>
+  </si>
+  <si>
+    <t>Call of Duty: Black Ops  Multiplayer</t>
+  </si>
+  <si>
+    <t>Day of Defeat: Source</t>
+  </si>
+  <si>
+    <t>DiRT 3</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>prediction</t>
+  </si>
+  <si>
+    <t>pctile</t>
+  </si>
+  <si>
+    <t>CounterStrike: Source</t>
+  </si>
+  <si>
+    <t>CounterStrike: Global Offensive</t>
+  </si>
+  <si>
+    <t>Call of Duty: Modern Warfare 3  Multiplayer</t>
+  </si>
+  <si>
+    <t>Rust</t>
+  </si>
+  <si>
+    <t>Source SDK</t>
+  </si>
+  <si>
+    <t>Call of Duty: Modern Warfare 3</t>
+  </si>
+  <si>
+    <t>Arma 2: Operation Arrowhead</t>
+  </si>
+  <si>
+    <t>HalfLife 2: Deathmatch</t>
+  </si>
+  <si>
+    <t>Sniper: Ghost Warrior</t>
+  </si>
+  <si>
+    <t>Arma 2</t>
+  </si>
+  <si>
+    <t>Arma 2: Private Military Company</t>
+  </si>
+  <si>
+    <t>playtime</t>
+  </si>
+  <si>
+    <t>steamid</t>
+  </si>
+  <si>
+    <t>Plants vs. Zombies: Game of the Year</t>
+  </si>
+  <si>
+    <t>Zuma's Revenge</t>
+  </si>
+  <si>
+    <t>Bookworm Adventures Deluxe</t>
+  </si>
+  <si>
+    <t>Insaniquarium! Deluxe</t>
+  </si>
+  <si>
+    <t>AstroPop Deluxe</t>
+  </si>
+  <si>
+    <t>Amazing Adventures Around the World</t>
+  </si>
+  <si>
+    <t>Chuzzle Deluxe</t>
+  </si>
+  <si>
+    <t>Dynomite! Deluxe</t>
+  </si>
+  <si>
+    <t>Hammer Heads Deluxe</t>
+  </si>
+  <si>
+    <t>Rocket Mania!</t>
+  </si>
+  <si>
+    <t>Typer Shark! Deluxe</t>
+  </si>
+  <si>
+    <t>Venice</t>
+  </si>
+  <si>
+    <t>Bejeweled Twist</t>
+  </si>
+  <si>
+    <t>The Wizard's Pen</t>
+  </si>
+  <si>
+    <t>Zuma Deluxe</t>
+  </si>
+  <si>
+    <t>Peggle Deluxe</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Feeding Frenzy 2: Shipwreck Showdown Deluxe</t>
+  </si>
+  <si>
+    <t>Big Money! Deluxe</t>
+  </si>
+  <si>
+    <t>Escape Rosecliff Island</t>
+  </si>
+  <si>
+    <t>Pizza Frenzy</t>
+  </si>
+  <si>
+    <t>Talismania Deluxe</t>
+  </si>
+  <si>
+    <t>Mystery P.I.: The Lottery Ticket</t>
+  </si>
+  <si>
+    <t>Heavy Weapon Deluxe</t>
+  </si>
+  <si>
+    <t>Iggle Pop! Deluxe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -100,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +258,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF37474F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -145,6 +299,33 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58568E53-3D6F-4E8E-919C-B0904F84BE93}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -883,4 +1064,585 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F325209-DF0D-4A60-9096-C62D3E207333}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>84086</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <v>183.46666666666701</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="9">
+        <v>30.0833333333333</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="9">
+        <v>21.6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <v>7.95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <v>2.7333333333333298</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>1.9653974100947401E-2</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3862.0166666666701</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>1.2675912119448201E-2</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="C12" s="9">
+        <v>170.61666666666699</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>4.7956132330000401E-3</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="C13" s="9">
+        <v>9.5333333333333297</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>1.60503352526575E-3</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C14" s="9">
+        <v>10.516666666666699</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>7.5501645915210204E-4</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="C15" s="9">
+        <v>3.1666666666666701</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>5.3333723917603504E-4</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C16" s="9">
+        <v>5.8666666666666698</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>3.8762559415772601E-4</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>3.5930427839048201E-4</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="C18" s="9">
+        <v>3</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>1.05689949123189E-4</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0.72</v>
+      </c>
+      <c r="C19" s="9">
+        <v>10.5833333333333</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>6.1140301113482605E-5</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>9.1714118752861395E-6</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0.96</v>
+      </c>
+      <c r="C21" s="9">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4635EE52-D0EF-4B3F-9A64-17A8E196423C}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="16">
+        <v>1751.31666666667</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16">
+        <v>639.29999999999995</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="9">
+        <v>24.05</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <v>9.0166666666666693</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <v>1.6666666666666701</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="9">
+        <v>1.31666666666667</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="9">
+        <v>0.68333333333333302</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="9">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="9">
+        <v>0.116666666666667</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="9">
+        <v>0.116666666666667</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="9">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>4.8135210818145397E-5</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="C20" s="9">
+        <v>3.56666666666667</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>7.2198977250082003E-6</v>
+      </c>
+      <c r="B21" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>1.9277827050245799E-6</v>
+      </c>
+      <c r="B22" s="10">
+        <v>0.82</v>
+      </c>
+      <c r="C22" s="9">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>6.3408685946342302E-7</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0.86</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2.81666666666667</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>4.1964068486777298E-7</v>
+      </c>
+      <c r="B24" s="15">
+        <v>0.88</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1338.4833333333299</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>3.7655445339623802E-7</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="C25" s="9">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>3.0072808954173498E-7</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0.92</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2.2333333333333298</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>1.935528928243E-7</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0.94</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>1.1891293638655E-7</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0.96</v>
+      </c>
+      <c r="C28" s="9">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>1.18727598419355E-7</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="C29" s="9">
+        <v>6.6666666666666693E-2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>9.8252364466588902E-8</v>
+      </c>
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A18:D18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cambios en tamanos de imagenes
</commit_message>
<xml_diff>
--- a/resultados_magic_loop.xlsx
+++ b/resultados_magic_loop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhnk7\Documents\MarioHeredia\ITAM\02_segundo_semestre\metodos_analiticos\final_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A199E400-67BB-4B34-BFA9-4B2319807862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9910D655-1EEF-4164-BC60-E68F56445BBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3DEE28E-3B65-4326-AC3A-6EBCD7C32232}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3DEE28E-3B65-4326-AC3A-6EBCD7C32232}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -207,7 +207,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -225,23 +225,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF37474F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFE0E0E0"/>
+      <color rgb="FF37474F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FFE0E0E0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FF37474F"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -257,13 +257,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF37474F"/>
+        <fgColor rgb="FFE0E0E0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,51 +281,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,8 +337,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE0E0E0"/>
       <color rgb="FF37474F"/>
-      <color rgb="FFE0E0E0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -649,391 +651,391 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58568E53-3D6F-4E8E-919C-B0904F84BE93}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="5" width="11.42578125" style="16"/>
+    <col min="6" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="16">
         <v>20</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17">
         <v>0.269823333805076</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="16">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16">
         <v>150</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="17">
         <v>0.18295871258253901</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="16">
         <v>20</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16">
         <v>500</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="17">
         <v>0.25376789055466897</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="16">
         <v>20</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="16">
         <v>20</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="17">
         <v>0.42510850114119603</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="16">
         <v>80</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17">
         <v>0.25131672506324298</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="16">
         <v>80</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="C7" s="16">
         <v>150</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="17">
         <v>0.173027776111745</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="16">
         <v>80</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="C8" s="16">
         <v>500</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="17">
         <v>0.24848058102368201</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="16">
         <v>80</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="16">
         <v>20</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="16">
         <v>150</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="17">
         <v>0.18498817748035601</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="16">
         <v>80</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="16">
         <v>40</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="16">
         <v>150</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="17">
         <v>0.201922820011356</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="16">
         <v>80</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="16">
         <v>40</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="16">
         <v>250</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="17">
         <v>0.193472568132491</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="16">
         <v>160</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B12" s="16">
+        <v>1</v>
+      </c>
+      <c r="C12" s="16">
         <v>150</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="17">
         <v>0.17120080209427199</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="16">
         <v>160</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16">
         <v>250</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="17">
         <v>0.17736296367433699</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="16">
         <v>160</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="16">
         <v>10</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="16">
         <v>150</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="17">
         <v>0.179447570871474</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="16">
         <v>160</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="16">
         <v>10</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="16">
         <v>250</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="17">
         <v>0.179871113014204</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19">
         <v>160</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="19">
         <v>80</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="19">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="A22" s="19">
+        <v>1</v>
+      </c>
+      <c r="B22" s="19">
+        <v>1</v>
+      </c>
+      <c r="C22" s="15">
         <v>0.24901951950000001</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="15">
         <v>0.25131672506324298</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="15">
         <v>0.269823333805076</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="19">
         <v>20</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="B23" s="19">
+        <v>1</v>
+      </c>
+      <c r="C23" s="15">
         <v>0.371</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5">
+      <c r="D23" s="15"/>
+      <c r="E23" s="15">
         <v>0.42510850114119603</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="19">
+        <v>1</v>
+      </c>
+      <c r="B24" s="19">
         <v>150</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="15">
         <v>0.17120080209427199</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="15">
         <v>0.173027776111745</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="15">
         <v>0.18295871258253901</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="19">
         <v>10</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="19">
         <v>150</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="15">
         <v>0.179447570871474</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="19">
         <v>20</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="19">
         <v>150</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15">
         <v>0.18498817748035601</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="19">
         <v>40</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="19">
         <v>150</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15">
         <v>0.201922820011356</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>1</v>
-      </c>
-      <c r="B28" s="4">
+      <c r="A28" s="19">
+        <v>1</v>
+      </c>
+      <c r="B28" s="19">
         <v>250</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="15">
         <v>0.17736296367433699</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+      <c r="A29" s="19">
         <v>10</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="19">
         <v>250</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="15">
         <v>0.179871113014204</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="19">
         <v>40</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="19">
         <v>250</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5">
+      <c r="C30" s="15"/>
+      <c r="D30" s="15">
         <v>0.193472568132491</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
-        <v>1</v>
-      </c>
-      <c r="B31" s="4">
+      <c r="A31" s="19">
+        <v>1</v>
+      </c>
+      <c r="B31" s="19">
         <v>500</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="15">
         <v>0.246789616203203</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="15">
         <v>0.24848058102368201</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="15">
         <v>0.25376789055466897</v>
       </c>
     </row>
@@ -1056,8 +1058,8 @@
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFE0E0E0"/>
         <color theme="0"/>
-        <color rgb="FFE0E0E0"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1070,249 +1072,280 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F325209-DF0D-4A60-9096-C62D3E207333}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D7"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="4"/>
+    <col min="2" max="2" width="13.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="4"/>
+    <col min="4" max="4" width="38.42578125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="G1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>84086</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="9">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="8">
         <v>183.46666666666701</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="9">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8">
         <v>30.0833333333333</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="9">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8">
         <v>21.6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="9">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="8">
         <v>7.95</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="9">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="8">
         <v>2.7333333333333298</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="10">
         <v>1.9653974100947401E-2</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="11">
         <v>0</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>3862.0166666666701</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <v>1.2675912119448201E-2</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="11">
         <v>0.02</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>170.61666666666699</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="10">
         <v>4.7956132330000401E-3</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="11">
         <v>0.04</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>9.5333333333333297</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="10">
         <v>1.60503352526575E-3</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>10.516666666666699</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="10">
         <v>7.5501645915210204E-4</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="11">
         <v>0.22</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>3.1666666666666701</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="10">
         <v>5.3333723917603504E-4</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>5.8666666666666698</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="10">
         <v>3.8762559415772601E-4</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="11">
         <v>0.32</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>0.05</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="10">
         <v>3.5930427839048201E-4</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="11">
         <v>0.36</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>3</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="10">
         <v>1.05689949123189E-4</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="11">
         <v>0.72</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>10.5833333333333</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="10">
         <v>6.1140301113482605E-5</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="11">
         <v>0.9</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>0.133333333333333</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A21" s="10">
         <v>9.1714118752861395E-6</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="11">
         <v>0.96</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A9:D9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1321,320 +1354,318 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4635EE52-D0EF-4B3F-9A64-17A8E196423C}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="11.42578125" style="6"/>
+    <col min="4" max="4" width="43.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="16">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
         <v>1751.31666666667</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="16">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
         <v>639.29999999999995</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>24.05</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>9.0166666666666693</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>1.6666666666666701</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>1.31666666666667</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>0.68333333333333302</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.16666666666666699</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>0.15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>0.116666666666667</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>0.116666666666667</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>0.1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>1.6666666666666701E-2</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="13">
         <v>4.8135210818145397E-5</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="11">
         <v>0.12</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>3.56666666666667</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="13">
         <v>7.2198977250082003E-6</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="11">
         <v>0.57999999999999996</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>0.133333333333333</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="13">
         <v>1.9277827050245799E-6</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="11">
         <v>0.82</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="13">
         <v>6.3408685946342302E-7</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="11">
         <v>0.86</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>2.81666666666667</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>4.1964068486777298E-7</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="3">
         <v>0.88</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="2">
         <v>1338.4833333333299</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="13">
         <v>3.7655445339623802E-7</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="11">
         <v>0.9</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>6.6666666666666693E-2</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="13">
         <v>3.0072808954173498E-7</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="11">
         <v>0.92</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8">
         <v>2.2333333333333298</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="13">
         <v>1.935528928243E-7</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="11">
         <v>0.94</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <v>0.15</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="13">
         <v>1.1891293638655E-7</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="11">
         <v>0.96</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>3.3333333333333298E-2</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="13">
         <v>1.18727598419355E-7</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="11">
         <v>0.98</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>6.6666666666666693E-2</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="13">
         <v>9.8252364466588902E-8</v>
       </c>
-      <c r="B30" s="10">
-        <v>1</v>
-      </c>
-      <c r="C30" s="9">
+      <c r="B30" s="11">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
         <v>0.05</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="6" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>